<commit_message>
merged from ppu test branch
</commit_message>
<xml_diff>
--- a/doc/de1-memory-doc.xlsx
+++ b/doc/de1-memory-doc.xlsx
@@ -2,19 +2,18 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="mem size" sheetId="1" r:id="rId1"/>
+    <sheet name="vga ppu architecture" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>NES required memory block</t>
   </si>
@@ -85,9 +84,6 @@
     <t>vga screen size</t>
   </si>
   <si>
-    <t>800 * 600 (w/ unvisible area)</t>
-  </si>
-  <si>
     <t>n/a</t>
   </si>
   <si>
@@ -101,6 +97,15 @@
   </si>
   <si>
     <t>bit</t>
+  </si>
+  <si>
+    <t>set ppu register</t>
+  </si>
+  <si>
+    <t>nmi exception</t>
+  </si>
+  <si>
+    <t>800 * 525 (w/ unvisible area)</t>
   </si>
 </sst>
 </file>
@@ -164,6 +169,707 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rounded Rectangle 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1190625" y="571500"/>
+          <a:ext cx="1666875" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>CPU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>44</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rounded Rectangle 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238750" y="571500"/>
+          <a:ext cx="5238750" cy="3048000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 3212"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>PPU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2857500" y="1333500"/>
+          <a:ext cx="2381250" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rounded Rectangle 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3095625" y="2476500"/>
+          <a:ext cx="1666875" cy="1143000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>chr rom</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>40</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rounded Rectangle 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7858125" y="1562100"/>
+          <a:ext cx="1666875" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>name/attr tble</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rounded Rectangle 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5762625" y="1562100"/>
+          <a:ext cx="1666875" cy="723900"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>palette tble</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>166689</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>204789</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Elbow Connector 9"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="8" idx="2"/>
+          <a:endCxn id="16" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="5886451" y="2995612"/>
+          <a:ext cx="2409825" cy="990600"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>204789</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>119064</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="11" name="Elbow Connector 10"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="7" idx="2"/>
+          <a:endCxn id="16" idx="0"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="6934201" y="2938462"/>
+          <a:ext cx="2409825" cy="1104900"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="15" name="Straight Connector 14"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="6" idx="3"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4762500" y="3048000"/>
+          <a:ext cx="1905000" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Rounded Rectangle 15"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6276976" y="4695825"/>
+          <a:ext cx="2619374" cy="1524000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>NTSC pixel</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> image</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>pixel rate=2.83 us</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>frame rate=30 Hz</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="24" name="Straight Connector 23"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="8" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238750" y="1333500"/>
+          <a:ext cx="523875" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="25" name="Straight Connector 24"/>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="7" idx="1"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5238750" y="1333500"/>
+          <a:ext cx="2619375" cy="590550"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:prstDash val="dash"/>
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>119064</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="29" name="Elbow Connector 28"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="3" idx="1"/>
+          <a:endCxn id="2" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="2024064" y="1714500"/>
+          <a:ext cx="3214687" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -417,7 +1123,31 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:spDef>
+      <a:spPr/>
+      <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+      <a:lstStyle>
+        <a:defPPr algn="l">
+          <a:defRPr sz="1100"/>
+        </a:defPPr>
+      </a:lstStyle>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </a:style>
+    </a:spDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
@@ -431,8 +1161,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,7 +1178,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="H3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -467,7 +1197,7 @@
         <v>45344</v>
       </c>
       <c r="I4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -486,7 +1216,7 @@
         <v>362752</v>
       </c>
       <c r="I5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -550,7 +1280,7 @@
         <v>5</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -574,10 +1304,10 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -588,24 +1318,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="N7:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="AO28" sqref="AO28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="7" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="O7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="14:15" x14ac:dyDescent="0.25">
+      <c r="N11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
memory map document update
</commit_message>
<xml_diff>
--- a/doc/de1-memory-doc.xlsx
+++ b/doc/de1-memory-doc.xlsx
@@ -1,23 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motooka\Documents\001-proj\999.my-proj\001.nes-fpga\repo\motonesfpga\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="11025" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="mem size" sheetId="1" r:id="rId1"/>
     <sheet name="vga ppu architecture" sheetId="2" r:id="rId2"/>
+    <sheet name="memory map" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -25,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="84">
   <si>
     <t>NES required memory block</t>
   </si>
@@ -106,17 +102,254 @@
   </si>
   <si>
     <t>800 * 525 (w/ unvisible area)</t>
+  </si>
+  <si>
+    <t>PRG-ROM upper bank</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PRG-ROM lower bank</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>SRAM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Expansion ROM</t>
+  </si>
+  <si>
+    <t>I/O registers</t>
+  </si>
+  <si>
+    <t>RAM</t>
+  </si>
+  <si>
+    <t>RAM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Stack</t>
+  </si>
+  <si>
+    <t>Zero page</t>
+  </si>
+  <si>
+    <t>0x10000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0100</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0200</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x4020</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x6000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x8000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0xC000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2008</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mirrors (2000 - 2007)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x4000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mirrors (0000 - 07FFF)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x0800</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CPU memory map</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PPU memory map</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sprite palette</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BG palette</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Att tbl 3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name tbl 3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Att tbl 2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name tbl 2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Attr tbl 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name tbl 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Attr tbl 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Name tbl 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pattern tbl 0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Pattern tbl 1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x1000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x3F20</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x3F10</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x3F00</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x3000</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2FC0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2C00</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2BC0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2800</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x27C0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x2400</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>0x23C0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mirros (2000 - 2EFF)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mirrors (3F00 -- 3F1F)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Mirrors (0000 - 3FFF)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PRG-ROM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>IO port</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>VRAM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>CHR ROM</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Palette RAM</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="6"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -135,7 +368,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -143,20 +376,89 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="dotted">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -872,6 +1174,341 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="右中かっこ 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3667125" y="819150"/>
+          <a:ext cx="238125" cy="2028825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>390525</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>57150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="右中かっこ 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3562350" y="5638800"/>
+          <a:ext cx="238125" cy="2828925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>638175</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="右中かっこ 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3571875" y="3876675"/>
+          <a:ext cx="238125" cy="1647825"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="右中かっこ 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8210550" y="3009900"/>
+          <a:ext cx="238125" cy="3895725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>647700</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="右中かっこ 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8210550" y="6915150"/>
+          <a:ext cx="238125" cy="1590675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="右中かっこ 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8220075" y="1828800"/>
+          <a:ext cx="238125" cy="1114425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rightBrace">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 100333"/>
+            <a:gd name="adj2" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -915,7 +1552,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -950,7 +1587,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1151,37 +1788,37 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A2:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.375" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="H3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1200,7 +1837,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1219,10 +1856,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9">
       <c r="D6" s="1"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="B7" t="s">
         <v>2</v>
       </c>
@@ -1238,7 +1875,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="B9" t="s">
         <v>4</v>
       </c>
@@ -1253,7 +1890,7 @@
         <v>2048</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="C10" t="s">
         <v>11</v>
       </c>
@@ -1264,7 +1901,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="C11" t="s">
         <v>8</v>
       </c>
@@ -1275,7 +1912,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="B13" t="s">
         <v>5</v>
       </c>
@@ -1283,13 +1920,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" s="2" customFormat="1"/>
+    <row r="18" spans="2:4">
       <c r="B18" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="C19" t="s">
         <v>16</v>
       </c>
@@ -1297,12 +1934,12 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="C22" t="s">
         <v>20</v>
       </c>
@@ -1311,33 +1948,404 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="N7:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AO28" sqref="AO28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="3.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="3.625" defaultRowHeight="13.5"/>
   <sheetData>
-    <row r="7" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="14:15">
       <c r="O7" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="14:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="14:15">
       <c r="N11" t="s">
         <v>25</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="B2:G49"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5"/>
+  <cols>
+    <col min="2" max="2" width="32.625" customWidth="1"/>
+    <col min="4" max="4" width="19.125" customWidth="1"/>
+    <col min="5" max="5" width="32.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="21">
+      <c r="B2" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7">
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7">
+      <c r="B5" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7">
+      <c r="B6" s="5"/>
+      <c r="E6" s="5"/>
+    </row>
+    <row r="7" spans="2:7">
+      <c r="B7" s="5"/>
+      <c r="E7" s="5"/>
+    </row>
+    <row r="8" spans="2:7">
+      <c r="B8" s="5"/>
+      <c r="E8" s="5"/>
+    </row>
+    <row r="9" spans="2:7">
+      <c r="B9" s="5"/>
+      <c r="E9" s="5"/>
+    </row>
+    <row r="10" spans="2:7">
+      <c r="B10" s="7"/>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7">
+      <c r="B11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7">
+      <c r="B12" s="5"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="2:7">
+      <c r="B13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7">
+      <c r="B14" s="5"/>
+      <c r="E14" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" s="6"/>
+      <c r="C16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" s="5"/>
+      <c r="E18" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" s="6"/>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7">
+      <c r="B21" s="5"/>
+      <c r="E21" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7">
+      <c r="B22" s="6"/>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7">
+      <c r="B23" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7">
+      <c r="B24" s="5"/>
+      <c r="E24" s="5"/>
+    </row>
+    <row r="25" spans="2:7">
+      <c r="B25" s="7"/>
+      <c r="C25" t="s">
+        <v>47</v>
+      </c>
+      <c r="E25" s="5"/>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7">
+      <c r="B26" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7">
+      <c r="B27" s="5"/>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="B28" s="5"/>
+      <c r="E28" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7">
+      <c r="B29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="G29" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7">
+      <c r="B30" s="7"/>
+      <c r="C30" t="s">
+        <v>45</v>
+      </c>
+      <c r="E30" s="5"/>
+      <c r="F30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7">
+      <c r="B31" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E31" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7">
+      <c r="B32" s="6"/>
+      <c r="C32" t="s">
+        <v>40</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7">
+      <c r="B33" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7">
+      <c r="B34" s="5"/>
+      <c r="E34" s="5"/>
+    </row>
+    <row r="35" spans="2:7">
+      <c r="B35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7">
+      <c r="B36" s="5"/>
+      <c r="E36" s="9" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7">
+      <c r="B37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7">
+      <c r="B38" s="5"/>
+      <c r="E38" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7">
+      <c r="B39" s="7"/>
+      <c r="C39" t="s">
+        <v>49</v>
+      </c>
+      <c r="E39" s="5"/>
+    </row>
+    <row r="40" spans="2:7">
+      <c r="B40" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7">
+      <c r="B41" s="5"/>
+      <c r="D41" t="s">
+        <v>33</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7">
+      <c r="B42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="2:7">
+      <c r="B43" s="6"/>
+      <c r="C43" t="s">
+        <v>39</v>
+      </c>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="2:7">
+      <c r="B44" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7">
+      <c r="B45" s="5"/>
+      <c r="E45" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="G45" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7">
+      <c r="B46" s="6"/>
+      <c r="C46" t="s">
+        <v>38</v>
+      </c>
+      <c r="E46" s="5"/>
+    </row>
+    <row r="47" spans="2:7">
+      <c r="B47" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="E47" s="5"/>
+    </row>
+    <row r="48" spans="2:7">
+      <c r="B48" s="5"/>
+      <c r="E48" s="5"/>
+    </row>
+    <row r="49" spans="2:6">
+      <c r="B49" s="6"/>
+      <c r="C49" t="s">
+        <v>37</v>
+      </c>
+      <c r="E49" s="6"/>
+      <c r="F49" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>